<commit_message>
docs: data structure update
</commit_message>
<xml_diff>
--- a/Proposal/Data structures.xlsx
+++ b/Proposal/Data structures.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\codeworks 2\exercise-pairs 2nd part\thesis-project-proposal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\codeworks 2\exercise-pairs 2nd part\thesisProjectBackend\Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
     <sheet name="User" sheetId="2" r:id="rId2"/>
+    <sheet name="Recommendation" sheetId="5" r:id="rId3"/>
+    <sheet name="Rating" sheetId="3" r:id="rId4"/>
+    <sheet name="routes" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>Product</t>
   </si>
@@ -142,13 +145,85 @@
   </si>
   <si>
     <t>[]</t>
+  </si>
+  <si>
+    <t>[id1, id2, …]</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>id1</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>id2</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/user</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>/product</t>
+  </si>
+  <si>
+    <t>/product/:id</t>
+  </si>
+  <si>
+    <t>/products/:categoryID/:subCategoryID</t>
+  </si>
+  <si>
+    <t>recommendation</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>/products/:recommendationID</t>
+  </si>
+  <si>
+    <t>used in</t>
+  </si>
+  <si>
+    <t>Future profile user Screen</t>
+  </si>
+  <si>
+    <t>Create product Screen</t>
+  </si>
+  <si>
+    <t>Register Screen</t>
+  </si>
+  <si>
+    <t>Product detail Screen</t>
+  </si>
+  <si>
+    <t>Category Screen</t>
+  </si>
+  <si>
+    <t>Home Screen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,13 +231,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -174,10 +263,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -185,8 +275,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F18"/>
+  <dimension ref="A2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +571,7 @@
     <col min="6" max="6" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -489,7 +582,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -497,7 +590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -508,7 +601,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>15</v>
       </c>
@@ -518,8 +611,11 @@
       <c r="F5" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -529,8 +625,11 @@
       <c r="F6" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -541,7 +640,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -552,7 +651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -563,7 +662,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -573,8 +672,11 @@
       <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -585,7 +687,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -596,7 +698,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -607,7 +709,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -617,8 +719,11 @@
       <c r="F14" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -628,8 +733,11 @@
       <c r="F15" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -640,7 +748,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -651,7 +759,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>14</v>
       </c>
@@ -660,6 +768,9 @@
       </c>
       <c r="F18" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="G18" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -669,10 +780,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F17"/>
+  <dimension ref="A2:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +792,7 @@
     <col min="6" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -692,7 +803,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -700,7 +811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -711,7 +822,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -722,7 +833,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -733,7 +844,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>
@@ -744,7 +855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>28</v>
       </c>
@@ -755,7 +866,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -766,7 +877,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -777,7 +888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -788,7 +899,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -799,7 +910,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -809,8 +920,11 @@
       <c r="F13" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>24</v>
       </c>
@@ -820,8 +934,11 @@
       <c r="F14" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -831,8 +948,11 @@
       <c r="F15" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>22</v>
       </c>
@@ -842,13 +962,226 @@
       <c r="F16" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="17" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="35.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>